<commit_message>
Updated schedules model, allow schedule patch on post
</commit_message>
<xml_diff>
--- a/src/assets/GenerationTemplates/weekday.xlsx
+++ b/src/assets/GenerationTemplates/weekday.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91420F2-44B5-EA43-9C71-74315C09DF77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6410486E-1607-EA4D-9F52-9965FF8B6984}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Edwaleni" sheetId="1" r:id="rId1"/>
@@ -1064,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B12:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
@@ -2545,8 +2545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B12:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3027,10 +3027,7 @@
         <f>SUM(F33:F40)</f>
         <v>0</v>
       </c>
-      <c r="I40" s="31">
-        <f>SUM(F35:F40)</f>
-        <v>0</v>
-      </c>
+      <c r="I40" s="31"/>
       <c r="J40" s="14"/>
     </row>
     <row r="41" spans="2:11" ht="15" x14ac:dyDescent="0.2">

</xml_diff>